<commit_message>
Adding test files and fixes to paged content template
</commit_message>
<xml_diff>
--- a/templates/CREATE/paged object ingest/Paged_Object_Ingest_Template.xlsx
+++ b/templates/CREATE/paged object ingest/Paged_Object_Ingest_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agaylie/Documents/GitHub/arca-templates/templates/CREATE/paged-compound object ingest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agaylie/Desktop/Arca Templates/june 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03107DB6-EDE0-F04D-AA68-3A6C49645EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2755F749-D4DE-F94B-8845-FF4B54120BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51620" yWindow="4000" windowWidth="36640" windowHeight="21100" xr2:uid="{C9DC37A4-3DAE-4B4E-8444-0766A02E0B8B}"/>
+    <workbookView xWindow="1560" yWindow="4300" windowWidth="43920" windowHeight="21980" xr2:uid="{C9DC37A4-3DAE-4B4E-8444-0766A02E0B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="294">
   <si>
     <t>ContentType</t>
   </si>
@@ -698,9 +698,6 @@
       </rPr>
       <t>. Separate multiple values with a pipe |</t>
     </r>
-  </si>
-  <si>
-    <t>4 pages</t>
   </si>
   <si>
     <t>PeerReviewStatus</t>
@@ -1154,22 +1151,7 @@
     </r>
   </si>
   <si>
-    <t>The Swedish Press - January 21, 1943</t>
-  </si>
-  <si>
-    <t>Vancouver (B.C.):1943-01-21:Central Press Limited</t>
-  </si>
-  <si>
     <t>newspaper</t>
-  </si>
-  <si>
-    <t>language:Swedish</t>
-  </si>
-  <si>
-    <t>Materials provided for research and reference use only. Permission to publish, copy, or otherwise use these materials must be obtained from Swedish Heritage in BC (refer to https://swedishheritagebc.ca) or the respective author/creator of the work.</t>
-  </si>
-  <si>
-    <t>The Swedish Press - January 28, 1943</t>
   </si>
   <si>
     <r>
@@ -1184,6 +1166,33 @@
       </rPr>
       <t>Node ID or URL alias of the parent object this child object will be going into (e.g., newspaper or compound parent). Node ID is recommended for a faster ingest.</t>
     </r>
+  </si>
+  <si>
+    <t>The White Rock Sun - April 17, 1958</t>
+  </si>
+  <si>
+    <t>The White Rock Sun - September 25, 1958</t>
+  </si>
+  <si>
+    <t>Materials provided for research and reference use only. Permission to publish, copy, or otherwise use these materials must be obtained from the White Rock Museum &amp; Archives.</t>
+  </si>
+  <si>
+    <t>language:English</t>
+  </si>
+  <si>
+    <t>3 pages</t>
+  </si>
+  <si>
+    <t>White Rock (B.C.):1958-04-17:Atkinson and Izowsky</t>
+  </si>
+  <si>
+    <t>White Rock (B.C.):1958-09-25:Atkinson and Izowsky</t>
+  </si>
+  <si>
+    <t>This is an excerpt for testing purposes only. Please visit https://bchdp.arcabc.ca/islandora/object/whiterock%3A6840 to view the full newspaper issue.</t>
+  </si>
+  <si>
+    <t>This is an excerpt for testing purposes only. Please visit https://bchdp.arcabc.ca/islandora/object/whiterock%3A6513 to view the full newspaper issue.</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1308,7 +1317,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1653,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0BA5A5-D0F6-DD43-B7E2-90723EE16CD6}">
   <dimension ref="A1:BT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AN15" sqref="AN15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1736,7 +1744,7 @@
         <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>95</v>
@@ -1951,214 +1959,214 @@
     </row>
     <row r="2" spans="1:72" s="6" customFormat="1" ht="152" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="Q2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="AO2" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="AN2" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AP2" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AP2" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="AQ2" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>213</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AT2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="AV2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="AY2" s="2" t="s">
+      <c r="BA2" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="AZ2" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BB2" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="BC2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="BD2" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="BC2" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="BD2" s="9" t="s">
+      <c r="BE2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="BF2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="BE2" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="BF2" s="2" t="s">
+      <c r="BG2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="BH2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="BG2" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BI2" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="BI2" s="9" t="s">
+      <c r="BK2" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="BM2" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="BJ2" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="BL2" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BN2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BP2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="BP2" s="2" t="s">
+      <c r="BQ2" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="BR2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="BQ2" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="BR2" s="2" t="s">
+      <c r="BS2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="BS2" s="2" t="s">
+      <c r="BT2" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="BT2" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:72" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -2166,12 +2174,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="10">
-        <v>15727</v>
+        <v>21292</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="P3" s="11"/>
+        <v>285</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>166</v>
       </c>
@@ -2179,22 +2195,22 @@
         <v>179</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>214</v>
+        <v>289</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="AN3" s="12">
-        <v>12345</v>
+        <v>288</v>
+      </c>
+      <c r="AN3" s="11">
+        <v>61</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="BE3" s="1" t="s">
         <v>80</v>
@@ -2203,7 +2219,7 @@
         <v>202</v>
       </c>
       <c r="BS3" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="BT3" s="1" t="s">
         <v>193</v>
@@ -2214,12 +2230,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="10">
-        <v>15734</v>
+        <v>21453</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="P4" s="11"/>
+        <v>286</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="Q4" s="1" t="s">
         <v>166</v>
       </c>
@@ -2227,22 +2251,22 @@
         <v>179</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>214</v>
+        <v>289</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="AN4" s="12">
-        <v>12345</v>
+        <v>288</v>
+      </c>
+      <c r="AN4" s="11">
+        <v>61</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="BE4" s="1" t="s">
         <v>80</v>
@@ -2251,7 +2275,7 @@
         <v>202</v>
       </c>
       <c r="BS4" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="BT4" s="1" t="s">
         <v>193</v>
@@ -2266,73 +2290,73 @@
           <x14:formula1>
             <xm:f>ControlledFields!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>M5:M1048576</xm:sqref>
+          <xm:sqref>M3:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38905BD2-FF57-8146-9B91-4B6D9FBE0736}">
           <x14:formula1>
             <xm:f>ControlledFields!$C$2:$C$46</xm:f>
           </x14:formula1>
-          <xm:sqref>K5:K1048576</xm:sqref>
+          <xm:sqref>K3:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38B4417C-5E4E-3341-8B8C-2F92AABDBA3B}">
           <x14:formula1>
             <xm:f>ControlledFields!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Q5:Q1048576</xm:sqref>
+          <xm:sqref>Q3:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60AA4061-909D-6F42-8165-5AE6FDD9092E}">
           <x14:formula1>
             <xm:f>ControlledFields!$H$2:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>R5:R1048576</xm:sqref>
+          <xm:sqref>R3:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0657D9BC-742E-054D-9D2F-3E547F362937}">
           <x14:formula1>
             <xm:f>ControlledFields!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>BC5:BC1048576</xm:sqref>
+          <xm:sqref>BC3:BC1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C2BD7472-7689-CB42-BDD2-2E526901459A}">
           <x14:formula1>
             <xm:f>ControlledFields!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>AO5:AO1048576</xm:sqref>
+          <xm:sqref>AO3:AO1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50171FF7-8052-B540-83BD-A7265DB72337}">
           <x14:formula1>
             <xm:f>ControlledFields!$J$2:$J$10</xm:f>
           </x14:formula1>
-          <xm:sqref>BO5:BO1048576</xm:sqref>
+          <xm:sqref>BO3:BO1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D0F90A4-A4E7-714F-994E-0D9C7460E024}">
           <x14:formula1>
             <xm:f>ControlledFields!$D$2:$D$13</xm:f>
           </x14:formula1>
-          <xm:sqref>BG5:BG1048576</xm:sqref>
+          <xm:sqref>BG3:BG1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4348959-A2A0-A848-A23F-88D2B9E30EA3}">
           <x14:formula1>
             <xm:f>ControlledFields!$E$2:$E$9</xm:f>
           </x14:formula1>
-          <xm:sqref>BT5:BT1048576</xm:sqref>
+          <xm:sqref>BT3:BT1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{856AC1A0-E17F-9B4A-AE30-253BBDEFA3BF}">
           <x14:formula1>
             <xm:f>ControlledFields!$K$2</xm:f>
           </x14:formula1>
-          <xm:sqref>AS5:AS1048576</xm:sqref>
+          <xm:sqref>AS3:AS1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCF8DC06-E2F1-BC4B-B3A5-233C0792FED6}">
           <x14:formula1>
             <xm:f>ControlledFields!$B$2:$B$34</xm:f>
           </x14:formula1>
-          <xm:sqref>BE5:BE1048576</xm:sqref>
+          <xm:sqref>BE3:BE1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{80E61061-89DE-1F43-8E42-22A922814FA9}">
           <x14:formula1>
             <xm:f>ControlledFields!$L$2:$L$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E5:E1048576</xm:sqref>
+          <xm:sqref>E3:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2344,8 +2368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071DE06A-0D68-D94A-AE87-43FCE8BE41B5}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2396,10 +2420,10 @@
         <v>184</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2437,7 +2461,7 @@
         <v>168</v>
       </c>
       <c r="L2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2472,7 +2496,7 @@
         <v>186</v>
       </c>
       <c r="L3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2507,7 +2531,7 @@
         <v>187</v>
       </c>
       <c r="L4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2533,7 +2557,7 @@
         <v>188</v>
       </c>
       <c r="L5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated descriptions for link text
Updated the descriptions for fields with links and link text (field_identifier_uri and field_url)
</commit_message>
<xml_diff>
--- a/templates/CREATE/paged object ingest/Paged_Object_Ingest_Template.xlsx
+++ b/templates/CREATE/paged object ingest/Paged_Object_Ingest_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agaylie/Desktop/Arca Templates/june 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agaylie/Documents/GitHub/arca-templates/templates/CREATE/paged object ingest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2755F749-D4DE-F94B-8845-FF4B54120BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285FF1C6-1349-DC40-BDB0-4701CA4625B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="4300" windowWidth="43920" windowHeight="21980" xr2:uid="{C9DC37A4-3DAE-4B4E-8444-0766A02E0B8B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="295">
   <si>
     <t>ContentType</t>
   </si>
@@ -1193,6 +1193,9 @@
   </si>
   <si>
     <t>This is an excerpt for testing purposes only. Please visit https://bchdp.arcabc.ca/islandora/object/whiterock%3A6513 to view the full newspaper issue.</t>
+  </si>
+  <si>
+    <t>mods_relation_types:preceding^The Semiahmoo Sun^https://bchdp.arcabc.ca/islandora/object/whiterock%3A1%%The Semiahmoo Sun 1940-1947^^newspaper^whiterock:1</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0BA5A5-D0F6-DD43-B7E2-90723EE16CD6}">
   <dimension ref="A1:BT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BD5" sqref="BD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2169,7 +2172,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:72" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2212,6 +2215,9 @@
       <c r="AO3" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="BD3" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="BE3" s="1" t="s">
         <v>80</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:72" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:72" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2268,6 +2274,9 @@
       <c r="AO4" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="BD4" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="BE4" s="1" t="s">
         <v>80</v>
       </c>
@@ -2283,6 +2292,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">

</xml_diff>